<commit_message>
Added revised Subjective assessment of reproducibility
Added revised version of subjective assessments, as of 17-09
</commit_message>
<xml_diff>
--- a/other-data/Subjective assessment of reproducibility.xlsx
+++ b/other-data/Subjective assessment of reproducibility.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kleber.INSTITUTO\Dropbox\Brazilian Reproducibility Initiative\Análise\Kleber\bri-analysis\other-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFE899F-0018-4D40-9C86-02A15BDE05B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA95BB7E-F559-AF48-A14A-CC9AAB2770C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="740" windowWidth="26060" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -426,9 +426,6 @@
     <t>EPM9</t>
   </si>
   <si>
-    <t>Condições locais distintas, animais diferentes, houve período de reforma predial nas facilidades aqui durante os esperimentos. Experimentadores diferentes, pequena diferença de idade e peso em relação ao artigo original.</t>
-  </si>
-  <si>
     <t>Comparando os nossos resultados com os originais, eles diferem entre si.</t>
   </si>
   <si>
@@ -1053,12 +1050,6 @@
   </si>
   <si>
     <t>LAB56</t>
-  </si>
-  <si>
-    <t>O perfil da resposta foi o mesmo, mas as amplitudes diferiram muito. No artigo original o aumento em resposta ao tratmento foi de 500% e no nosso caso foi de 5.000%</t>
-  </si>
-  <si>
-    <t>Além da qualidade dos primers pois nossas melting não ficaram boas para nenhum dos genes, talvez a qualidade do soro</t>
   </si>
   <si>
     <t>Os eluentes dos reagentes foram diferentes do protocolo original</t>
@@ -1727,12 +1718,21 @@
   <si>
     <t>Justificativa: Diferenças</t>
   </si>
+  <si>
+    <t xml:space="preserve">O fato de, em nosso laboratório, o IC incluir o 100%. </t>
+  </si>
+  <si>
+    <t>1) Mais de um pico na melting curve do normalizador e do gene de interesse (principalmente neste); 2) Obtivemos um aumento significativo do grupo DMSO diferenciado em relação ao controle branco não diferenciado e uma diminuição significativa do tratado não diferenciado comparado com o DMSO diferenciado (oposto do descrito no artigo)</t>
+  </si>
+  <si>
+    <t>1) falha na diferenciação completa das células; 2) desenho de primers favorecendo dimerização cruzada; 3) qualidade de síntese dos primers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1745,6 +1745,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1767,12 +1773,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1968,18 +1975,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="14" width="18.85546875" customWidth="1"/>
+    <col min="1" max="14" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1990,10 +1997,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2002,10 +2009,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2026,7 +2033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2050,7 +2057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2074,7 +2081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2098,7 +2105,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2122,7 +2129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -2146,7 +2153,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -2191,7 +2198,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -2215,7 +2222,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -2236,7 +2243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -2260,7 +2267,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -2281,7 +2288,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -2305,7 +2312,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -2329,7 +2336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -2353,7 +2360,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -2377,7 +2384,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
@@ -2401,7 +2408,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -2425,7 +2432,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
@@ -2449,7 +2456,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>81</v>
       </c>
@@ -2473,7 +2480,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>81</v>
       </c>
@@ -2497,7 +2504,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>89</v>
       </c>
@@ -2518,7 +2525,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
@@ -2542,7 +2549,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>89</v>
       </c>
@@ -2566,7 +2573,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>100</v>
       </c>
@@ -2590,7 +2597,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>100</v>
       </c>
@@ -2614,7 +2621,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
@@ -2638,7 +2645,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>100</v>
       </c>
@@ -2662,7 +2669,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="332" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>117</v>
       </c>
@@ -2685,7 +2692,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="331.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="319" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>117</v>
       </c>
@@ -2708,7 +2715,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>126</v>
       </c>
@@ -2718,136 +2725,136 @@
       <c r="C32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G32" s="1">
         <v>2</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G33" s="1">
         <v>2</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G34" s="1">
         <v>2</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="G35" s="1">
         <v>2</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G36" s="1">
         <v>3</v>
       </c>
       <c r="H36" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
@@ -2857,12 +2864,12 @@
         <v>2</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>113</v>
@@ -2871,46 +2878,46 @@
         <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G38" s="1">
         <v>2</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G39" s="1">
         <v>2</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>38</v>
@@ -2919,7 +2926,7 @@
         <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
@@ -2929,12 +2936,12 @@
         <v>4</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>45</v>
@@ -2943,22 +2950,22 @@
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G41" s="1">
         <v>1</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>118</v>
@@ -2967,22 +2974,22 @@
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>109</v>
@@ -2991,22 +2998,22 @@
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G43" s="1">
         <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>90</v>
@@ -3015,112 +3022,112 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G45" s="1">
         <v>2</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E46" s="1"/>
       <c r="G46" s="1">
         <v>3</v>
       </c>
       <c r="H46" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G47" s="1">
         <v>4</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E48" s="1"/>
       <c r="G48" s="1">
         <v>3</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>109</v>
@@ -3129,40 +3136,40 @@
         <v>7</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E49" s="1"/>
       <c r="G49" s="1">
         <v>3</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E50" s="1"/>
       <c r="G50" s="1">
         <v>1</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>85</v>
@@ -3171,22 +3178,22 @@
         <v>7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G51" s="1">
         <v>1</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>57</v>
@@ -3195,22 +3202,22 @@
         <v>11</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G52" s="1">
         <v>2</v>
       </c>
       <c r="H52" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>10</v>
@@ -3219,70 +3226,70 @@
         <v>11</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G53" s="1">
         <v>2</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G54" s="1">
         <v>2</v>
       </c>
       <c r="H54" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G55" s="1">
         <v>2</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>90</v>
@@ -3291,22 +3298,22 @@
         <v>11</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G56" s="1">
         <v>2</v>
       </c>
       <c r="H56" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A57" s="1" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>53</v>
@@ -3315,115 +3322,115 @@
         <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G57" s="1">
         <v>1</v>
       </c>
       <c r="H57" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G58" s="1">
         <v>5</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A59" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G59" s="1">
         <v>2</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G60" s="1">
         <v>2</v>
       </c>
       <c r="H60" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="371" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="408" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E61" s="1"/>
       <c r="G61" s="1">
         <v>2</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="408" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>50</v>
@@ -3432,115 +3439,115 @@
         <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G62" s="1">
         <v>5</v>
       </c>
       <c r="H62" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G63" s="1">
         <v>4</v>
       </c>
       <c r="H63" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="E64" s="1"/>
       <c r="G64" s="1">
         <v>2</v>
       </c>
       <c r="H64" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>245</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G65" s="1">
         <v>3</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G66" s="1">
         <v>1</v>
       </c>
       <c r="H66" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>122</v>
@@ -3549,67 +3556,67 @@
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E67" s="1"/>
       <c r="G67" s="1">
         <v>1</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G68" s="1">
         <v>1</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="B69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G69" s="1">
         <v>1</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>77</v>
@@ -3618,22 +3625,22 @@
         <v>11</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
       </c>
       <c r="H70" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>50</v>
@@ -3642,46 +3649,46 @@
         <v>7</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G71" s="1">
         <v>2</v>
       </c>
       <c r="H71" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G72" s="1">
         <v>1</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>101</v>
@@ -3690,24 +3697,24 @@
         <v>11</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="F73" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="G73" s="1">
         <v>5</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>57</v>
@@ -3716,160 +3723,160 @@
         <v>11</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G74" s="1">
         <v>2</v>
       </c>
       <c r="H74" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="154" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="153" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E75" s="1"/>
       <c r="G75" s="1">
         <v>1</v>
       </c>
       <c r="H75" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="345" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="331.5" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G76" s="1">
         <v>1</v>
       </c>
       <c r="H76" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A77" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G77" s="1">
         <v>1</v>
       </c>
       <c r="H77" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A78" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+      <c r="B78" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>292</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G78" s="1">
         <v>1</v>
       </c>
       <c r="H78" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G79" s="1">
         <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E80" s="1"/>
       <c r="G80" s="1">
         <v>2</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>93</v>
@@ -3878,208 +3885,208 @@
         <v>11</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G81" s="1">
         <v>5</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A82" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="B82" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E82" s="1"/>
       <c r="G82" s="1">
         <v>2</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E83" s="1"/>
       <c r="G83" s="1">
         <v>2</v>
       </c>
       <c r="H83" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A84" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="B84" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G84" s="1">
         <v>1</v>
       </c>
       <c r="H84" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A85" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G85" s="1">
         <v>1</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G86" s="1">
         <v>1</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G87" s="1">
         <v>1</v>
       </c>
       <c r="H87" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A88" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G88" s="1">
         <v>1</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>327</v>
+        <v>242</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>510</v>
       </c>
       <c r="E89" s="1"/>
-      <c r="F89" s="1" t="s">
-        <v>328</v>
+      <c r="F89" s="3" t="s">
+        <v>511</v>
       </c>
       <c r="G89" s="1">
         <v>2</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>101</v>
@@ -4088,94 +4095,94 @@
         <v>7</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G90" s="1">
         <v>3</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G91" s="1">
         <v>1</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G92" s="1">
         <v>1</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G93" s="1">
         <v>5</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>105</v>
@@ -4184,31 +4191,31 @@
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G94" s="1">
         <v>5</v>
       </c>
       <c r="H94" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="280" x14ac:dyDescent="0.15">
+      <c r="A95" s="1" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="267.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="B95" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
@@ -4218,60 +4225,60 @@
         <v>1</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G97" s="1">
         <v>2</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>20</v>
@@ -4280,43 +4287,43 @@
         <v>11</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E98" s="1"/>
       <c r="G98" s="1">
         <v>5</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G99" s="1">
         <v>2</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>118</v>
@@ -4325,112 +4332,112 @@
         <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E100" s="1"/>
       <c r="G100" s="1">
         <v>3</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E101" s="1"/>
       <c r="G101" s="1">
         <v>3</v>
       </c>
       <c r="H101" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A102" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>365</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
       </c>
       <c r="H102" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A103" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>370</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G103" s="1">
         <v>3</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G104" s="1">
         <v>3</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>127</v>
@@ -4439,19 +4446,19 @@
         <v>7</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E105" s="1"/>
       <c r="G105" s="1">
         <v>1</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>20</v>
@@ -4460,162 +4467,162 @@
         <v>11</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G106" s="1">
         <v>3</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G107" s="1">
         <v>1</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G108" s="1">
         <v>1</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G109" s="1">
         <v>1</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G110" s="1">
         <v>1</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E111" s="1"/>
       <c r="G111" s="1">
         <v>1</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G112" s="1">
         <v>1</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>85</v>
@@ -4624,22 +4631,22 @@
         <v>11</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G113" s="1">
         <v>3</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>16</v>
@@ -4648,24 +4655,24 @@
         <v>11</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G114" s="1">
         <v>3</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>27</v>
@@ -4674,48 +4681,48 @@
         <v>11</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E115" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>410</v>
       </c>
       <c r="G115" s="1">
         <v>2</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G116" s="1">
         <v>2</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>38</v>
@@ -4724,43 +4731,43 @@
         <v>7</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="E117" s="1"/>
       <c r="G117" s="1">
         <v>1</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G118" s="1">
         <v>1</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>127</v>
@@ -4769,48 +4776,48 @@
         <v>11</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G119" s="1">
         <v>2</v>
       </c>
       <c r="H119" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A120" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F120" s="1" t="s">
         <v>424</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>427</v>
       </c>
       <c r="G120" s="1">
         <v>3</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>66</v>
@@ -4819,70 +4826,70 @@
         <v>11</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G121" s="1">
         <v>2</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G122" s="1">
         <v>2</v>
       </c>
       <c r="H122" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="319" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>434</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="293.25" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>437</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G123" s="1">
         <v>2</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>27</v>
@@ -4891,46 +4898,46 @@
         <v>11</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G124" s="1">
         <v>2</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G125" s="1">
         <v>1</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>66</v>
@@ -4939,163 +4946,163 @@
         <v>11</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G126" s="1">
         <v>2</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E127" s="1"/>
       <c r="G127" s="1">
         <v>2</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>452</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G128" s="1">
         <v>3</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G129" s="1">
         <v>1</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="G130" s="1">
         <v>1</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G131" s="1">
         <v>5</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G132" s="1">
         <v>1</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>24</v>
@@ -5104,72 +5111,72 @@
         <v>11</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G133" s="1">
         <v>2</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G134" s="1">
         <v>4</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G135" s="1">
         <v>2</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>16</v>
@@ -5178,46 +5185,46 @@
         <v>11</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G136" s="1">
         <v>2</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G137" s="1">
         <v>2</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>62</v>
@@ -5226,22 +5233,22 @@
         <v>11</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G138" s="1">
         <v>2</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>24</v>
@@ -5250,91 +5257,91 @@
         <v>11</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="G139" s="1">
         <v>2</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="G140" s="1">
         <v>2</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E141" s="1"/>
       <c r="G141" s="1">
         <v>4</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G142" s="1">
         <v>2</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>122</v>
@@ -5343,22 +5350,22 @@
         <v>11</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="G143" s="1">
         <v>3</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>30</v>
@@ -5367,7 +5374,7 @@
         <v>7</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
@@ -5377,7 +5384,7 @@
         <v>2</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated inclusion sets and subjective analysis
Inclusion sets contains n=1 experiments and (for now) breaks power simulations.
Revised post-hoc power values and added inclusion set for >80% power in bigexp
</commit_message>
<xml_diff>
--- a/other-data/Subjective assessment of reproducibility.xlsx
+++ b/other-data/Subjective assessment of reproducibility.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4928E5-775E-3743-8C47-A61ED88ABD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6861E228-84C6-4B4C-A117-09FAB31E502B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="740" windowWidth="26060" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="740" windowWidth="26060" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -519,15 +519,6 @@
     <t>O cultivo celular teve que ser interpretado pelo nosso grupo e o grupo da IBR (Bruna, principalmente) pois a descrição nos Materirias e Métodos é confusa. Os primers descritos para amplificação de CD90 não amplificam o gene descrito, após avaliação tivemos que alterar um dos primers para poder amplificar o gene CD90. Mesmo assim, este par de primer não se mostrou ótimo para o realizar qPCR, embora funcione bem para em gel de agarose.</t>
   </si>
   <si>
-    <t>nossos dados não apresentaram diferenças entre MPP+ e MPP+Cannabidiol</t>
-  </si>
-  <si>
-    <t>Embora a parte experimental foi perfeitamente replicada, com controles funcionando de forma igual (controle MPP+ produzindo a metade do sinal do controle não tratado), o tratamento com cannabidiol não reverteu o efeito do MPP+. Segundo a literatura a absorbância do MTT, na concentração usada de MPP+, deve ser de aproximadamente a metade do que nas células não tratadas. Ao avaliar a figura 4A, vemos que, mesmo tratadas com cannabidiol, a absorbância relativa ficou perto dos 50%. Um explicação pode ser que nossos dados tem desvio maior do que o sugerido pela fig 4 e isto influenciou no fato do grupo tratado não apresentar diferênça estatística com o grupo MPP+.</t>
-  </si>
-  <si>
-    <t>Concentrações de reagentes e tempos seguiram exatamente os métodos do artigo e os controles se comportaram de acordo com os dados apresentados pelo artigo.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Embora a descrição do artigo permite entender como replicar o experimento, nossos dados não permitem ver diferença estatística na expressão do gene ABCC1 entre controle e tratados. </t>
   </si>
   <si>
@@ -787,9 +778,6 @@
   </si>
   <si>
     <t>PCR139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O experimento original mostra que após 8h de hipóxia as células passam a expressar mais VEGF-A. Ao realizarmos o experimento, com n=8 de experimentos independentes, notamos que a variação de expressão do marcador era muito oscilante, perdendo poder estatístico. Alguns pontos devem ser levantados: em nosso experimento, o saquinho de Hipóxia não era o mesmo, o que pode ter feito com que a vedação total não fosse possível. O artigo diz que foram realizadas triplicatas, mas não explicam de quantos poços, e quantas passagens foram realizadas entre elas. </t>
   </si>
   <si>
     <t>Além dos pontos citados acima, não podemos descartar o fato da falta de rotina de nosso laboratório na manipulação desse tipo celular e desse experimento proposto. Além do mais, por atrasos nas empresas de entregas, nos restaram pouquíssimo tempo para realização do experimento, não podendo realizar testes e/ou padronizações anteriores.</t>
@@ -1726,6 +1714,18 @@
   </si>
   <si>
     <t>O fato de o experimento original ter comprovado a diferenciação das células já é o principal fator, que muda todo o resultado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não observamos diferença estatística entre o grupo tratado e o veículo. </t>
+  </si>
+  <si>
+    <t>No artigo original (Fig. 4), nota-se que as células SCC9 tratadas (10 µM) apresentam um aumento para valores próximos a 170%. No entanto, não é detalhado se este resultado corresponde a 6, 24 ou 48 horas — os três tempos descritos na legenda da figura. Embora o corpo do texto indique que o gráfico se refere às 6 horas de tratamento (mencionando que em 24 e 48 horas não houve diferença estatística), é difícil explicar um aumento de 70% que não se sustenta ou não apresenta continuidade nos tempos subsequentes. Essa inconsistência nos leva a questionar a robustez metodológica dos autores.</t>
+  </si>
+  <si>
+    <t>não tivemos mudanças no sistema de cultivo, pequenas alterações foram feitas no protocolo do MTT quanto à solubilização dos cristais formados no ensaio de MTT, mas isto não deveria alterar os dados obtidos para os diferentes tratamentos.</t>
+  </si>
+  <si>
+    <t>Após uma análise correta dos resultados (os quais tínhamos lido de forma invertida devido a falta o sinal no expoente do 2-deltadeltaCt), cremos que o experimento não teve uma correta replicação, ou seja, o gene PIPKIIa não teve aumento de expressão nas células tratadas</t>
   </si>
 </sst>
 </file>
@@ -1978,7 +1978,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1997,10 +1997,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2009,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -2467,7 +2467,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2475,7 +2475,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
@@ -2724,7 +2724,7 @@
         <v>11</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>125</v>
@@ -2947,18 +2947,18 @@
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>159</v>
+      <c r="D41" s="3" t="s">
+        <v>508</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1" t="s">
-        <v>160</v>
+      <c r="F41" s="3" t="s">
+        <v>509</v>
       </c>
       <c r="G41" s="1">
         <v>1</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>161</v>
+      <c r="H41" s="3" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.15">
@@ -2972,17 +2972,17 @@
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.15">
@@ -2996,17 +2996,17 @@
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G43" s="1">
         <v>2</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
@@ -3020,17 +3020,17 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.15">
@@ -3038,94 +3038,94 @@
         <v>156</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G45" s="1">
         <v>2</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E46" s="1"/>
       <c r="G46" s="1">
         <v>3</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G47" s="1">
         <v>4</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E48" s="1"/>
       <c r="G48" s="1">
         <v>3</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>106</v>
@@ -3134,40 +3134,40 @@
         <v>7</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E49" s="1"/>
       <c r="G49" s="1">
         <v>3</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E50" s="1"/>
       <c r="G50" s="1">
         <v>1</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>82</v>
@@ -3176,22 +3176,22 @@
         <v>7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G51" s="1">
         <v>1</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>57</v>
@@ -3200,22 +3200,22 @@
         <v>11</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G52" s="1">
         <v>2</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>10</v>
@@ -3224,70 +3224,70 @@
         <v>11</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G53" s="1">
         <v>2</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G54" s="1">
         <v>2</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G55" s="1">
         <v>2</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>87</v>
@@ -3296,22 +3296,22 @@
         <v>11</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G56" s="1">
         <v>2</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>53</v>
@@ -3320,115 +3320,115 @@
         <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G57" s="1">
         <v>1</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G58" s="1">
         <v>5</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G59" s="1">
         <v>2</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G60" s="1">
         <v>2</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="371" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E61" s="1"/>
       <c r="G61" s="1">
         <v>2</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>50</v>
@@ -3437,49 +3437,49 @@
         <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G62" s="1">
         <v>5</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G63" s="1">
         <v>4</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -3488,69 +3488,69 @@
         <v>11</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="G64" s="3">
         <v>4</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>240</v>
+        <v>511</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G65" s="1">
         <v>3</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G66" s="1">
         <v>1</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>119</v>
@@ -3559,19 +3559,19 @@
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E67" s="1"/>
       <c r="G67" s="1">
         <v>1</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>146</v>
@@ -3580,46 +3580,46 @@
         <v>11</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G68" s="1">
         <v>1</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G69" s="1">
         <v>1</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>77</v>
@@ -3628,22 +3628,22 @@
         <v>11</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>50</v>
@@ -3652,46 +3652,46 @@
         <v>7</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G71" s="1">
         <v>2</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="G72" s="1">
         <v>1</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>98</v>
@@ -3700,24 +3700,24 @@
         <v>11</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G73" s="1">
         <v>5</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>57</v>
@@ -3726,160 +3726,160 @@
         <v>11</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G74" s="1">
         <v>2</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="154" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E75" s="1"/>
       <c r="G75" s="1">
         <v>1</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="345" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="C76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G76" s="1">
         <v>1</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G77" s="1">
         <v>1</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G78" s="1">
         <v>1</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G79" s="1">
         <v>1</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E80" s="1"/>
       <c r="G80" s="1">
         <v>2</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>90</v>
@@ -3888,208 +3888,208 @@
         <v>11</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G81" s="1">
         <v>5</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E82" s="1"/>
       <c r="G82" s="1">
         <v>2</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E83" s="1"/>
       <c r="G83" s="1">
         <v>2</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G84" s="1">
         <v>1</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G85" s="1">
         <v>1</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G86" s="1">
         <v>1</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G87" s="1">
         <v>1</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="G88" s="1">
         <v>1</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="3" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G89" s="1">
         <v>2</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>98</v>
@@ -4098,22 +4098,22 @@
         <v>7</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G90" s="1">
         <v>3</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>152</v>
@@ -4122,70 +4122,70 @@
         <v>11</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G91" s="1">
         <v>1</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G92" s="1">
         <v>1</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G93" s="1">
         <v>5</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>102</v>
@@ -4194,31 +4194,31 @@
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G94" s="1">
         <v>5</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="280" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
@@ -4228,36 +4228,36 @@
         <v>1</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>141</v>
@@ -4266,22 +4266,22 @@
         <v>7</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G97" s="1">
         <v>2</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>20</v>
@@ -4290,43 +4290,43 @@
         <v>11</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E98" s="1"/>
       <c r="G98" s="1">
         <v>5</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G99" s="1">
         <v>2</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>115</v>
@@ -4335,112 +4335,112 @@
         <v>7</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E100" s="1"/>
       <c r="G100" s="1">
         <v>3</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E101" s="1"/>
       <c r="G101" s="1">
         <v>3</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G103" s="1">
         <v>3</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G104" s="1">
         <v>3</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>124</v>
@@ -4449,19 +4449,19 @@
         <v>7</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E105" s="1"/>
       <c r="G105" s="1">
         <v>1</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>20</v>
@@ -4470,46 +4470,46 @@
         <v>11</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G106" s="1">
         <v>3</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G107" s="1">
         <v>1</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>136</v>
@@ -4518,22 +4518,22 @@
         <v>11</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G108" s="1">
         <v>1</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>128</v>
@@ -4542,90 +4542,90 @@
         <v>11</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G109" s="1">
         <v>1</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G110" s="1">
         <v>1</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="E111" s="1"/>
       <c r="G111" s="1">
         <v>1</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G112" s="1">
         <v>1</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>82</v>
@@ -4634,22 +4634,22 @@
         <v>11</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G113" s="1">
         <v>3</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>16</v>
@@ -4658,24 +4658,24 @@
         <v>11</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G114" s="1">
         <v>3</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>27</v>
@@ -4684,48 +4684,48 @@
         <v>11</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G115" s="1">
         <v>2</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G116" s="1">
         <v>2</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>38</v>
@@ -4734,19 +4734,19 @@
         <v>7</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E117" s="1"/>
       <c r="G117" s="1">
         <v>1</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>146</v>
@@ -4755,22 +4755,22 @@
         <v>11</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G118" s="1">
         <v>1</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>124</v>
@@ -4779,48 +4779,48 @@
         <v>11</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G119" s="1">
         <v>2</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="E120" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G120" s="1">
         <v>3</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>66</v>
@@ -4829,22 +4829,22 @@
         <v>11</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G121" s="1">
         <v>2</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>132</v>
@@ -4853,46 +4853,46 @@
         <v>11</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G122" s="1">
         <v>2</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="319" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G123" s="1">
         <v>2</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>27</v>
@@ -4901,46 +4901,46 @@
         <v>11</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="G124" s="1">
         <v>2</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G125" s="1">
         <v>1</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>66</v>
@@ -4949,22 +4949,22 @@
         <v>11</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G126" s="1">
         <v>2</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>141</v>
@@ -4973,139 +4973,139 @@
         <v>7</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E127" s="1"/>
       <c r="G127" s="1">
         <v>2</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G128" s="1">
         <v>3</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G129" s="1">
         <v>1</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G130" s="1">
         <v>1</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D131" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G131" s="1">
         <v>5</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G132" s="1">
         <v>1</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>24</v>
@@ -5114,48 +5114,48 @@
         <v>11</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="G133" s="1">
         <v>2</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G134" s="1">
         <v>4</v>
       </c>
       <c r="H134" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>136</v>
@@ -5164,22 +5164,22 @@
         <v>11</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G135" s="1">
         <v>2</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>16</v>
@@ -5188,46 +5188,46 @@
         <v>11</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G136" s="1">
         <v>2</v>
       </c>
       <c r="H136" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G137" s="1">
         <v>2</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>62</v>
@@ -5236,22 +5236,22 @@
         <v>11</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="G138" s="1">
         <v>2</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>24</v>
@@ -5260,91 +5260,91 @@
         <v>11</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G139" s="1">
         <v>2</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="G140" s="1">
         <v>2</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E141" s="1"/>
       <c r="G141" s="1">
         <v>4</v>
       </c>
       <c r="H141" s="2" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="G142" s="1">
         <v>2</v>
       </c>
       <c r="H142" s="2" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>119</v>
@@ -5353,22 +5353,22 @@
         <v>11</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="2" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="G143" s="1">
         <v>3</v>
       </c>
       <c r="H143" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>30</v>
@@ -5377,7 +5377,7 @@
         <v>7</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
@@ -5387,7 +5387,7 @@
         <v>2</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>